<commit_message>
Updated data and docs
Updated data and docs to the latest version from Study Direct. spec.pdf is now user_requirments.pdf.
</commit_message>
<xml_diff>
--- a/data/card_data.xlsx
+++ b/data/card_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Property Tycoon board data</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Player puts £50 on free parking</t>
   </si>
   <si>
-    <t>Back pays £100 to the player</t>
-  </si>
-  <si>
     <t>As the card says</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>"You have won a lip sync battle. Collect £100"</t>
   </si>
   <si>
-    <t>Back pays player £100</t>
-  </si>
-  <si>
     <t>"Advance to Turing Heights"</t>
   </si>
   <si>
@@ -198,6 +192,9 @@
   </si>
   <si>
     <t>"Advance to Skywalker Drive. If you pass GO collect £200"</t>
+  </si>
+  <si>
+    <t>Bank pays £100 to the player</t>
   </si>
 </sst>
 </file>
@@ -570,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824FCAE1-2E2D-480B-8168-72B223ADDCE7}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +604,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -687,47 +684,47 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
         <v>27</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
         <v>29</v>
-      </c>
-      <c r="D21" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -742,7 +739,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
         <v>19</v>
@@ -750,122 +747,122 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" t="s">
         <v>29</v>
-      </c>
-      <c r="D41" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>